<commit_message>
Fix: Incorrect legend and add important info about the test env
</commit_message>
<xml_diff>
--- a/MyWork/Threading_Performance.xlsx
+++ b/MyWork/Threading_Performance.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23610"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F1B6D65-D1E2-4107-910E-327D2C4F132D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1BA2C837-DC6F-4F7F-AA3D-45C051202BCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,18 +11,12 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$2:$A$21</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$F$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$F$2:$F$21</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$B$2:$B$21</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$C$2:$C$21</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$D$2:$D$21</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$E$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$E$2:$E$21</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$2:$A$21</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$2:$B$21</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$2:$C$21</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$D$2:$D$21</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$E$2:$E$21</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$F$2:$F$21</definedName>
   </definedNames>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
@@ -40,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>Sequential (.net 3.1)</t>
   </si>
@@ -59,12 +53,18 @@
   <si>
     <t>Parallel (.net 5.0)</t>
   </si>
+  <si>
+    <t>Note: My windows 10 is running in virtual machine and I was not allowed to change the affinity processor</t>
+  </si>
+  <si>
+    <t>Tested on virtual machine with 2 processor and 2 GB memory</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,6 +88,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -176,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -193,6 +201,7 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1096,32 +1105,32 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="4">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.4</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="5">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.11</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2421,8 +2430,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4248150" y="266700"/>
-              <a:ext cx="4572000" cy="2743200"/>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2752,9 +2761,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -3157,7 +3168,7 @@
       <c r="J19" t="s">
         <v>1</v>
       </c>
-      <c r="M19" s="8"/>
+      <c r="M19" s="9"/>
       <c r="N19" t="s">
         <v>4</v>
       </c>
@@ -3185,7 +3196,7 @@
       <c r="J20" t="s">
         <v>2</v>
       </c>
-      <c r="M20" s="9"/>
+      <c r="M20" s="8"/>
       <c r="N20" t="s">
         <v>5</v>
       </c>
@@ -3208,6 +3219,16 @@
       </c>
       <c r="F21" s="3">
         <v>151</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" s="10" customFormat="1">
+      <c r="A23" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>